<commit_message>
550 parsed tales, raw data
</commit_message>
<xml_diff>
--- a/data/raw/список_сказок.xlsx
+++ b/data/raw/список_сказок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\folk_art\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F59AA9-05FF-4833-BD29-73FC97E94EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9236C302-E6A5-4CA1-8708-8791FECF7997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="68" windowWidth="10155" windowHeight="11459" xr2:uid="{32319B73-5396-4F80-A1E8-48F64898489E}"/>
   </bookViews>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EE065C-7F43-4346-A617-098E22C2BBF6}">
   <dimension ref="A1:E551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A536" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B552" sqref="B552"/>
+    <sheetView tabSelected="1" topLeftCell="A546" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B557" sqref="B557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A390">
-        <f t="shared" ref="A390:A420" si="7">A389+1</f>
+        <f t="shared" ref="A390:A453" si="7">A389+1</f>
         <v>389</v>
       </c>
       <c r="B390" t="s">
@@ -6418,658 +6418,1575 @@
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A421">
+        <f t="shared" si="7"/>
+        <v>420</v>
+      </c>
       <c r="B421" t="s">
         <v>258</v>
       </c>
+      <c r="C421">
+        <v>1</v>
+      </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A422">
+        <f t="shared" si="7"/>
+        <v>421</v>
+      </c>
       <c r="B422" t="s">
         <v>258</v>
       </c>
+      <c r="C422">
+        <v>1</v>
+      </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A423">
+        <f t="shared" si="7"/>
+        <v>422</v>
+      </c>
       <c r="B423" t="s">
         <v>259</v>
       </c>
+      <c r="C423">
+        <v>1</v>
+      </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A424">
+        <f t="shared" si="7"/>
+        <v>423</v>
+      </c>
       <c r="B424" t="s">
         <v>259</v>
       </c>
+      <c r="C424">
+        <v>1</v>
+      </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A425">
+        <f t="shared" si="7"/>
+        <v>424</v>
+      </c>
       <c r="B425" t="s">
         <v>259</v>
       </c>
+      <c r="C425">
+        <v>1</v>
+      </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A426">
+        <f t="shared" si="7"/>
+        <v>425</v>
+      </c>
       <c r="B426" t="s">
         <v>120</v>
       </c>
+      <c r="C426">
+        <v>1</v>
+      </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A427">
+        <f t="shared" si="7"/>
+        <v>426</v>
+      </c>
       <c r="B427" t="s">
         <v>120</v>
       </c>
+      <c r="C427">
+        <v>1</v>
+      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A428">
+        <f t="shared" si="7"/>
+        <v>427</v>
+      </c>
       <c r="B428" t="s">
         <v>260</v>
       </c>
+      <c r="C428">
+        <v>1</v>
+      </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A429">
+        <f t="shared" si="7"/>
+        <v>428</v>
+      </c>
       <c r="B429" t="s">
         <v>261</v>
       </c>
+      <c r="C429">
+        <v>1</v>
+      </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A430">
+        <f t="shared" si="7"/>
+        <v>429</v>
+      </c>
       <c r="B430" t="s">
         <v>261</v>
       </c>
+      <c r="C430">
+        <v>1</v>
+      </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A431">
+        <f t="shared" si="7"/>
+        <v>430</v>
+      </c>
       <c r="B431" t="s">
         <v>262</v>
       </c>
+      <c r="C431">
+        <v>1</v>
+      </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A432">
+        <f t="shared" si="7"/>
+        <v>431</v>
+      </c>
       <c r="B432" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="433" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A433">
+        <f t="shared" si="7"/>
+        <v>432</v>
+      </c>
       <c r="B433" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A434">
+        <f t="shared" si="7"/>
+        <v>433</v>
+      </c>
       <c r="B434" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="435" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C434">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A435">
+        <f t="shared" si="7"/>
+        <v>434</v>
+      </c>
       <c r="B435" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="436" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A436">
+        <f t="shared" si="7"/>
+        <v>435</v>
+      </c>
       <c r="B436" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A437">
+        <f t="shared" si="7"/>
+        <v>436</v>
+      </c>
       <c r="B437" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="438" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C437">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A438">
+        <f t="shared" si="7"/>
+        <v>437</v>
+      </c>
       <c r="B438" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="439" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A439">
+        <f t="shared" si="7"/>
+        <v>438</v>
+      </c>
       <c r="B439" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A440">
+        <f t="shared" si="7"/>
+        <v>439</v>
+      </c>
       <c r="B440" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="441" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A441">
+        <f t="shared" si="7"/>
+        <v>440</v>
+      </c>
       <c r="B441" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="442" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A442">
+        <f t="shared" si="7"/>
+        <v>441</v>
+      </c>
       <c r="B442" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A443">
+        <f t="shared" si="7"/>
+        <v>442</v>
+      </c>
       <c r="B443" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="444" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A444">
+        <f t="shared" si="7"/>
+        <v>443</v>
+      </c>
       <c r="B444" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="445" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A445">
+        <f t="shared" si="7"/>
+        <v>444</v>
+      </c>
       <c r="B445" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A446">
+        <f t="shared" si="7"/>
+        <v>445</v>
+      </c>
       <c r="B446" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="447" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A447">
+        <f t="shared" si="7"/>
+        <v>446</v>
+      </c>
       <c r="B447" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="448" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A448">
+        <f t="shared" si="7"/>
+        <v>447</v>
+      </c>
       <c r="B448" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A449">
+        <f t="shared" si="7"/>
+        <v>448</v>
+      </c>
       <c r="B449" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="450" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A450">
+        <f t="shared" si="7"/>
+        <v>449</v>
+      </c>
       <c r="B450" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="451" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A451">
+        <f t="shared" si="7"/>
+        <v>450</v>
+      </c>
       <c r="B451" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="452" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A452">
+        <f t="shared" si="7"/>
+        <v>451</v>
+      </c>
       <c r="B452" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A453">
+        <f t="shared" si="7"/>
+        <v>452</v>
+      </c>
       <c r="B453" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="454" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A454">
+        <f t="shared" ref="A454:A517" si="8">A453+1</f>
+        <v>453</v>
+      </c>
       <c r="B454" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A455">
+        <f t="shared" si="8"/>
+        <v>454</v>
+      </c>
       <c r="B455" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A456">
+        <f t="shared" si="8"/>
+        <v>455</v>
+      </c>
       <c r="B456" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="457" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A457">
+        <f t="shared" si="8"/>
+        <v>456</v>
+      </c>
       <c r="B457" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="458" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A458">
+        <f t="shared" si="8"/>
+        <v>457</v>
+      </c>
       <c r="B458" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A459">
+        <f t="shared" si="8"/>
+        <v>458</v>
+      </c>
       <c r="B459" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="460" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A460">
+        <f t="shared" si="8"/>
+        <v>459</v>
+      </c>
       <c r="B460" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A461">
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
       <c r="B461" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A462">
+        <f t="shared" si="8"/>
+        <v>461</v>
+      </c>
       <c r="B462" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="463" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A463">
+        <f t="shared" si="8"/>
+        <v>462</v>
+      </c>
       <c r="B463" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="464" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A464">
+        <f t="shared" si="8"/>
+        <v>463</v>
+      </c>
       <c r="B464" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="465" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A465">
+        <f t="shared" si="8"/>
+        <v>464</v>
+      </c>
       <c r="B465" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="466" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A466">
+        <f t="shared" si="8"/>
+        <v>465</v>
+      </c>
       <c r="B466" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="467" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A467">
+        <f t="shared" si="8"/>
+        <v>466</v>
+      </c>
       <c r="B467" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="468" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A468">
+        <f t="shared" si="8"/>
+        <v>467</v>
+      </c>
       <c r="B468" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="469" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A469">
+        <f t="shared" si="8"/>
+        <v>468</v>
+      </c>
       <c r="B469" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="470" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A470">
+        <f t="shared" si="8"/>
+        <v>469</v>
+      </c>
       <c r="B470" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A471">
+        <f t="shared" si="8"/>
+        <v>470</v>
+      </c>
       <c r="B471" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="472" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A472">
+        <f t="shared" si="8"/>
+        <v>471</v>
+      </c>
       <c r="B472" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="473" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A473">
+        <f t="shared" si="8"/>
+        <v>472</v>
+      </c>
       <c r="B473" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="474" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A474">
+        <f t="shared" si="8"/>
+        <v>473</v>
+      </c>
       <c r="B474" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="475" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C474">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A475">
+        <f t="shared" si="8"/>
+        <v>474</v>
+      </c>
       <c r="B475" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="476" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C475">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A476">
+        <f t="shared" si="8"/>
+        <v>475</v>
+      </c>
       <c r="B476" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="477" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A477">
+        <f t="shared" si="8"/>
+        <v>476</v>
+      </c>
       <c r="B477" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="478" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C477">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A478">
+        <f t="shared" si="8"/>
+        <v>477</v>
+      </c>
       <c r="B478" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="479" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C478">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A479">
+        <f t="shared" si="8"/>
+        <v>478</v>
+      </c>
       <c r="B479" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="480" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A480">
+        <f t="shared" si="8"/>
+        <v>479</v>
+      </c>
       <c r="B480" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A481">
+        <f t="shared" si="8"/>
+        <v>480</v>
+      </c>
       <c r="B481" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C481">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A482">
+        <f t="shared" si="8"/>
+        <v>481</v>
+      </c>
       <c r="B482" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="483" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A483">
+        <f t="shared" si="8"/>
+        <v>482</v>
+      </c>
       <c r="B483" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="484" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C483">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A484">
+        <f t="shared" si="8"/>
+        <v>483</v>
+      </c>
       <c r="B484" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="485" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C484">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A485">
+        <f t="shared" si="8"/>
+        <v>484</v>
+      </c>
       <c r="B485" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="486" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A486">
+        <f t="shared" si="8"/>
+        <v>485</v>
+      </c>
       <c r="B486" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="487" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A487">
+        <f t="shared" si="8"/>
+        <v>486</v>
+      </c>
       <c r="B487" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="488" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A488">
+        <f t="shared" si="8"/>
+        <v>487</v>
+      </c>
       <c r="B488" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="489" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A489">
+        <f t="shared" si="8"/>
+        <v>488</v>
+      </c>
       <c r="B489" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A490">
+        <f t="shared" si="8"/>
+        <v>489</v>
+      </c>
       <c r="B490" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="491" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C490">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A491">
+        <f t="shared" si="8"/>
+        <v>490</v>
+      </c>
       <c r="B491" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="492" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A492">
+        <f t="shared" si="8"/>
+        <v>491</v>
+      </c>
       <c r="B492" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="493" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A493">
+        <f t="shared" si="8"/>
+        <v>492</v>
+      </c>
       <c r="B493" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="494" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A494">
+        <f t="shared" si="8"/>
+        <v>493</v>
+      </c>
       <c r="B494" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="495" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A495">
+        <f t="shared" si="8"/>
+        <v>494</v>
+      </c>
       <c r="B495" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="496" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A496">
+        <f t="shared" si="8"/>
+        <v>495</v>
+      </c>
       <c r="B496" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="497" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C496">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A497">
+        <f t="shared" si="8"/>
+        <v>496</v>
+      </c>
       <c r="B497" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="498" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C497">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A498">
+        <f t="shared" si="8"/>
+        <v>497</v>
+      </c>
       <c r="B498" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="499" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A499">
+        <f t="shared" si="8"/>
+        <v>498</v>
+      </c>
       <c r="B499" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="500" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A500">
+        <f t="shared" si="8"/>
+        <v>499</v>
+      </c>
       <c r="B500" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="501" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A501">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
       <c r="B501" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="502" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A502">
+        <f t="shared" si="8"/>
+        <v>501</v>
+      </c>
       <c r="B502" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="503" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C502">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A503">
+        <f t="shared" si="8"/>
+        <v>502</v>
+      </c>
       <c r="B503" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="504" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C503">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A504">
+        <f t="shared" si="8"/>
+        <v>503</v>
+      </c>
       <c r="B504" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="505" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C504">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A505">
+        <f t="shared" si="8"/>
+        <v>504</v>
+      </c>
       <c r="B505" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="506" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C505">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A506">
+        <f t="shared" si="8"/>
+        <v>505</v>
+      </c>
       <c r="B506" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="507" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A507">
+        <f t="shared" si="8"/>
+        <v>506</v>
+      </c>
       <c r="B507" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="508" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C507">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A508">
+        <f t="shared" si="8"/>
+        <v>507</v>
+      </c>
       <c r="B508" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="509" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C508">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A509">
+        <f t="shared" si="8"/>
+        <v>508</v>
+      </c>
       <c r="B509" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="510" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C509">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A510">
+        <f t="shared" si="8"/>
+        <v>509</v>
+      </c>
       <c r="B510" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="511" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A511">
+        <f t="shared" si="8"/>
+        <v>510</v>
+      </c>
       <c r="B511" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="512" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C511">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A512">
+        <f t="shared" si="8"/>
+        <v>511</v>
+      </c>
       <c r="B512" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="513" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A513">
+        <f t="shared" si="8"/>
+        <v>512</v>
+      </c>
       <c r="B513" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="514" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C513">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A514">
+        <f t="shared" si="8"/>
+        <v>513</v>
+      </c>
       <c r="B514" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="515" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A515">
+        <f t="shared" si="8"/>
+        <v>514</v>
+      </c>
       <c r="B515" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="516" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C515">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A516">
+        <f t="shared" si="8"/>
+        <v>515</v>
+      </c>
       <c r="B516" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="517" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C516">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A517">
+        <f t="shared" si="8"/>
+        <v>516</v>
+      </c>
       <c r="B517" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="518" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A518">
+        <f t="shared" ref="A518:A551" si="9">A517+1</f>
+        <v>517</v>
+      </c>
       <c r="B518" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="519" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C518">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A519">
+        <f t="shared" si="9"/>
+        <v>518</v>
+      </c>
       <c r="B519" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="520" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C519">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A520">
+        <f t="shared" si="9"/>
+        <v>519</v>
+      </c>
       <c r="B520" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="521" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A521">
+        <f t="shared" si="9"/>
+        <v>520</v>
+      </c>
       <c r="B521" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="522" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A522">
+        <f t="shared" si="9"/>
+        <v>521</v>
+      </c>
       <c r="B522" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="523" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A523">
+        <f t="shared" si="9"/>
+        <v>522</v>
+      </c>
       <c r="B523" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="524" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A524">
+        <f t="shared" si="9"/>
+        <v>523</v>
+      </c>
       <c r="B524" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="525" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C524">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A525">
+        <f t="shared" si="9"/>
+        <v>524</v>
+      </c>
       <c r="B525" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="526" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C525">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A526">
+        <f t="shared" si="9"/>
+        <v>525</v>
+      </c>
       <c r="B526" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="527" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C526">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A527">
+        <f t="shared" si="9"/>
+        <v>526</v>
+      </c>
       <c r="B527" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="528" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C527">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A528">
+        <f t="shared" si="9"/>
+        <v>527</v>
+      </c>
       <c r="B528" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A529">
+        <f t="shared" si="9"/>
+        <v>528</v>
+      </c>
       <c r="B529" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="530" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C529">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A530">
+        <f t="shared" si="9"/>
+        <v>529</v>
+      </c>
       <c r="B530" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C530">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A531">
+        <f t="shared" si="9"/>
+        <v>530</v>
+      </c>
       <c r="B531" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C531">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A532">
+        <f t="shared" si="9"/>
+        <v>531</v>
+      </c>
       <c r="B532" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="533" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C532">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A533">
+        <f t="shared" si="9"/>
+        <v>532</v>
+      </c>
       <c r="B533" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A534">
+        <f t="shared" si="9"/>
+        <v>533</v>
+      </c>
       <c r="B534" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C534">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A535">
+        <f t="shared" si="9"/>
+        <v>534</v>
+      </c>
       <c r="B535" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="536" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C535">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A536">
+        <f t="shared" si="9"/>
+        <v>535</v>
+      </c>
       <c r="B536" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C536">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A537">
+        <f t="shared" si="9"/>
+        <v>536</v>
+      </c>
       <c r="B537" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="538" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C537">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A538">
+        <f t="shared" si="9"/>
+        <v>537</v>
+      </c>
       <c r="B538" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C538">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A539">
+        <f t="shared" si="9"/>
+        <v>538</v>
+      </c>
       <c r="B539" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="540" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C539">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A540">
+        <f t="shared" si="9"/>
+        <v>539</v>
+      </c>
       <c r="B540" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A541">
+        <f t="shared" si="9"/>
+        <v>540</v>
+      </c>
       <c r="B541" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C541">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A542">
+        <f t="shared" si="9"/>
+        <v>541</v>
+      </c>
       <c r="B542" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C542">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A543">
+        <f t="shared" si="9"/>
+        <v>542</v>
+      </c>
       <c r="B543" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="544" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A544">
+        <f t="shared" si="9"/>
+        <v>543</v>
+      </c>
       <c r="B544" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="545" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A545">
+        <f t="shared" si="9"/>
+        <v>544</v>
+      </c>
       <c r="B545" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="546" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C545">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A546">
+        <f t="shared" si="9"/>
+        <v>545</v>
+      </c>
       <c r="B546" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="547" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C546">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A547">
+        <f t="shared" si="9"/>
+        <v>546</v>
+      </c>
       <c r="B547" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C547">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A548">
+        <f t="shared" si="9"/>
+        <v>547</v>
+      </c>
       <c r="B548" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C548">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A549">
+        <f t="shared" si="9"/>
+        <v>548</v>
+      </c>
       <c r="B549" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="550" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C549">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A550">
+        <f t="shared" si="9"/>
+        <v>549</v>
+      </c>
       <c r="B550" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="551" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="C550">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A551">
+        <f t="shared" si="9"/>
+        <v>550</v>
+      </c>
       <c r="B551" t="s">
         <v>318</v>
+      </c>
+      <c r="C551">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>